<commit_message>
Update private cloud, rekentijd model
* Private cloud kan worden aangeroepen met python scripts
* 'hashmaps' met energyflows die elke tijdstap gecleared en gevuld worden uitgezet tbv rekentijd
* Wat minder belangrijke aanpassingen in diverse excells en jsons gebruikt om te experimenteren met private cloud
</commit_message>
<xml_diff>
--- a/Base/Benchmark AnyLogic API.xlsx
+++ b/Base/Benchmark AnyLogic API.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F50074E-DF55-485C-92A1-6F65D870ABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A4CE73-402B-498D-B530-8AE2D41836F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E845474-1578-4D90-89CE-AD8BAB5BC2FA}"/>
+    <workbookView xWindow="5508" yWindow="3708" windowWidth="23040" windowHeight="12216" xr2:uid="{7E845474-1578-4D90-89CE-AD8BAB5BC2FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>responstijd API (s)</t>
   </si>
@@ -48,6 +47,9 @@
   </si>
   <si>
     <t>totaal agents</t>
+  </si>
+  <si>
+    <t>responsetijd private cloud</t>
   </si>
 </sst>
 </file>
@@ -496,6 +498,99 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0F7A-4F74-A40A-9A754F1C10ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>responsetijd private cloud</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5F73-4C00-811F-8570DFE1B4C6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -760,11 +855,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:legendEntry>
-        <c:idx val="2"/>
+        <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="3"/>
+        <c:idx val="4"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -1406,8 +1501,8 @@
       <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -1734,22 +1829,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F392E5EB-2CAF-4A57-B5FB-21CFD6EA24FB}">
-  <dimension ref="C2:F19"/>
+  <dimension ref="C2:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="15.625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1762,8 +1857,11 @@
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>28</v>
       </c>
@@ -1777,8 +1875,11 @@
       <c r="F3" s="4">
         <v>0.75</v>
       </c>
+      <c r="G3">
+        <v>5.4</v>
+      </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>300</v>
       </c>
@@ -1792,8 +1893,11 @@
       <c r="F4" s="4">
         <v>1.78</v>
       </c>
+      <c r="G4">
+        <v>6.2</v>
+      </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>1000</v>
       </c>
@@ -1807,8 +1911,11 @@
       <c r="F5">
         <v>2.5</v>
       </c>
+      <c r="G5">
+        <v>12.8</v>
+      </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Parallel processing of agent creation and calculation loops
*Configuration: o.a. default energy assets
Run: o.a. gridConnection calculateEnergyBalance(), connectionOwner updateFinances().
*Dummy-parameter voor forceren uncached cloud-runs met dezelfde instellingen
*Pythonscripts: modelkeuze wordt nu in experiment gemaakt; caching kan omzeild worden met boolean.
</commit_message>
<xml_diff>
--- a/Base/Benchmark AnyLogic API.xlsx
+++ b/Base/Benchmark AnyLogic API.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A4CE73-402B-498D-B530-8AE2D41836F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03900B9-5EAC-48CF-8950-28BA5762E5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5508" yWindow="3708" windowWidth="23040" windowHeight="12216" xr2:uid="{7E845474-1578-4D90-89CE-AD8BAB5BC2FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E845474-1578-4D90-89CE-AD8BAB5BC2FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>responstijd API (s)</t>
   </si>
@@ -50,6 +50,24 @@
   </si>
   <si>
     <t>responsetijd private cloud</t>
+  </si>
+  <si>
+    <t>privateCloud 16/9</t>
+  </si>
+  <si>
+    <t>t=1h</t>
+  </si>
+  <si>
+    <t>t=0.25h</t>
+  </si>
+  <si>
+    <t>Cloud parallel</t>
+  </si>
+  <si>
+    <t>private cloud cached</t>
+  </si>
+  <si>
+    <t>parallel default energyassets</t>
   </si>
 </sst>
 </file>
@@ -551,6 +569,21 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$C$3:$C$5</c:f>
@@ -591,6 +624,185 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5F73-4C00-811F-8570DFE1B4C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>privateCloud 16/9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9E3C-40CD-ABA8-F6C5BE0ED12D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cloud parallel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-9E3C-40CD-ABA8-F6C5BE0ED12D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -855,11 +1067,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:legendEntry>
-        <c:idx val="3"/>
+        <c:idx val="5"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="4"/>
+        <c:idx val="6"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -1495,16 +1707,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>491490</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>124776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>78105</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1829,22 +2041,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F392E5EB-2CAF-4A57-B5FB-21CFD6EA24FB}">
-  <dimension ref="C2:G19"/>
+  <dimension ref="C1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="18.125" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1860,8 +2080,20 @@
       <c r="G2" t="s">
         <v>4</v>
       </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>28</v>
       </c>
@@ -1878,8 +2110,23 @@
       <c r="G3">
         <v>5.4</v>
       </c>
+      <c r="H3">
+        <v>6.1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>6.05</v>
+      </c>
+      <c r="J3">
+        <v>11.8</v>
+      </c>
+      <c r="K3">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="L3">
+        <v>5.875</v>
+      </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>300</v>
       </c>
@@ -1896,8 +2143,23 @@
       <c r="G4">
         <v>6.2</v>
       </c>
+      <c r="H4">
+        <v>6.7</v>
+      </c>
+      <c r="I4" s="4">
+        <v>11.9</v>
+      </c>
+      <c r="J4">
+        <v>11.9</v>
+      </c>
+      <c r="K4">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="L4">
+        <v>6.85</v>
+      </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>1000</v>
       </c>
@@ -1914,8 +2176,26 @@
       <c r="G5">
         <v>12.8</v>
       </c>
+      <c r="H5">
+        <v>12.9</v>
+      </c>
+      <c r="I5" s="4">
+        <v>23.64</v>
+      </c>
+      <c r="J5">
+        <v>18.3</v>
+      </c>
+      <c r="K5">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="L5">
+        <v>7.3650000000000002</v>
+      </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>

</xml_diff>